<commit_message>
Add a new checkWording task to check wording validity (optional)
</commit_message>
<xml_diff>
--- a/sample/wording.xlsx
+++ b/sample/wording.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -29,36 +29,72 @@
     <t>ES</t>
   </si>
   <si>
+    <t>key6</t>
+  </si>
+  <si>
     <t>key1</t>
   </si>
   <si>
+    <t>Sample key 6</t>
+  </si>
+  <si>
     <t>Sample key 1</t>
   </si>
   <si>
     <t>Value 1</t>
   </si>
   <si>
+    <t>Value 6</t>
+  </si>
+  <si>
+    <t>Validated</t>
+  </si>
+  <si>
+    <t>Valeur 6</t>
+  </si>
+  <si>
     <t>Valeur 1</t>
   </si>
   <si>
+    <t>To validate</t>
+  </si>
+  <si>
     <t>Valor 1</t>
   </si>
   <si>
+    <t>Valor 6</t>
+  </si>
+  <si>
+    <t>key7</t>
+  </si>
+  <si>
     <t>key2</t>
   </si>
   <si>
+    <t>Sample key 7</t>
+  </si>
+  <si>
     <t>Sample key 2</t>
   </si>
   <si>
+    <t>Value 7</t>
+  </si>
+  <si>
     <t>Value 2</t>
   </si>
   <si>
+    <t>Valeur 7</t>
+  </si>
+  <si>
     <t>Valeur 2</t>
   </si>
   <si>
     <t>Valor 2</t>
   </si>
   <si>
+    <t>Valor 7</t>
+  </si>
+  <si>
     <t>key3</t>
   </si>
   <si>
@@ -71,9 +107,6 @@
     <t>Valor 3</t>
   </si>
   <si>
-    <t>key6</t>
-  </si>
-  <si>
     <t>key4</t>
   </si>
   <si>
@@ -83,24 +116,12 @@
     <t>Value 4</t>
   </si>
   <si>
-    <t>Sample key 6</t>
-  </si>
-  <si>
     <t>Valeur 4</t>
   </si>
   <si>
-    <t>Value 6</t>
-  </si>
-  <si>
     <t>Valor 4</t>
   </si>
   <si>
-    <t>Valeur 6</t>
-  </si>
-  <si>
-    <t>Valor 6</t>
-  </si>
-  <si>
     <t>key5</t>
   </si>
   <si>
@@ -110,22 +131,7 @@
     <t>Valeur 5</t>
   </si>
   <si>
-    <t>key7</t>
-  </si>
-  <si>
     <t>Valor 5</t>
-  </si>
-  <si>
-    <t>Sample key 7</t>
-  </si>
-  <si>
-    <t>Value 7</t>
-  </si>
-  <si>
-    <t>Valeur 7</t>
-  </si>
-  <si>
-    <t>Valor 7</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,32 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1C232"/>
+          <bgColor rgb="FFF1C232"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -212,93 +243,153 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D6 F2:F6 H2:H6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"To validate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D6 F2:F6 H2:H6">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Validated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D6 F2:F6 H2:H6">
+      <formula1>"To validate,Validated"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -326,48 +417,84 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D3 F2:F3 H2:H3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"To validate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3 F2:F3 H2:H3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Validated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D3 F2:F3 H2:H3">
+      <formula1>"To validate,Validated"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>